<commit_message>
Added 4th Plate Design
</commit_message>
<xml_diff>
--- a/data/Designs/Designs_masterfile.xlsx
+++ b/data/Designs/Designs_masterfile.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOL428\Documents\GitHub\SynBioMLMH\SynbioML\data\Designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E67AE20B-C96D-4C2D-9615-6DD57D4BB9EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4888FD7C-BA65-4DA9-82D4-BEDCA957CDBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="3350" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sequences" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1168" uniqueCount="725">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1618" uniqueCount="996">
   <si>
     <t>tttaagaaggagatatacat</t>
   </si>
@@ -2205,6 +2205,819 @@
   </si>
   <si>
     <t>Round</t>
+  </si>
+  <si>
+    <t>RBS_2008</t>
+  </si>
+  <si>
+    <t>RBS_1363</t>
+  </si>
+  <si>
+    <t>RBS_1765</t>
+  </si>
+  <si>
+    <t>RBS_1998</t>
+  </si>
+  <si>
+    <t>RBS_1300</t>
+  </si>
+  <si>
+    <t>RBS_1342</t>
+  </si>
+  <si>
+    <t>RBS_2134</t>
+  </si>
+  <si>
+    <t>RBS_2012</t>
+  </si>
+  <si>
+    <t>RBS_1352</t>
+  </si>
+  <si>
+    <t>RBS_2070</t>
+  </si>
+  <si>
+    <t>RBS_1986</t>
+  </si>
+  <si>
+    <t>RBS_1884</t>
+  </si>
+  <si>
+    <t>RBS_1367</t>
+  </si>
+  <si>
+    <t>RBS_2478</t>
+  </si>
+  <si>
+    <t>RBS_1348</t>
+  </si>
+  <si>
+    <t>RBS_1755</t>
+  </si>
+  <si>
+    <t>RBS_3714</t>
+  </si>
+  <si>
+    <t>RBS_2598</t>
+  </si>
+  <si>
+    <t>RBS_1304</t>
+  </si>
+  <si>
+    <t>RBS_1422</t>
+  </si>
+  <si>
+    <t>RBS_1369</t>
+  </si>
+  <si>
+    <t>RBS_2978</t>
+  </si>
+  <si>
+    <t>RBS_2112</t>
+  </si>
+  <si>
+    <t>RBS_2025</t>
+  </si>
+  <si>
+    <t>RBS_1373</t>
+  </si>
+  <si>
+    <t>RBS_2988</t>
+  </si>
+  <si>
+    <t>RBS_2620</t>
+  </si>
+  <si>
+    <t>RBS_1391</t>
+  </si>
+  <si>
+    <t>RBS_3051</t>
+  </si>
+  <si>
+    <t>RBS_1769</t>
+  </si>
+  <si>
+    <t>RBS_2060</t>
+  </si>
+  <si>
+    <t>RBS_2018</t>
+  </si>
+  <si>
+    <t>RBS_2118</t>
+  </si>
+  <si>
+    <t>RBS_1875</t>
+  </si>
+  <si>
+    <t>RBS_3704</t>
+  </si>
+  <si>
+    <t>RBS_1134</t>
+  </si>
+  <si>
+    <t>RBS_1354</t>
+  </si>
+  <si>
+    <t>RBS_2608</t>
+  </si>
+  <si>
+    <t>RBS_3442</t>
+  </si>
+  <si>
+    <t>RBS_2124</t>
+  </si>
+  <si>
+    <t>RBS_2966</t>
+  </si>
+  <si>
+    <t>RBS_1292</t>
+  </si>
+  <si>
+    <t>RBS_2074</t>
+  </si>
+  <si>
+    <t>RBS_1358</t>
+  </si>
+  <si>
+    <t>RBS_2028</t>
+  </si>
+  <si>
+    <t>RBS_1380</t>
+  </si>
+  <si>
+    <t>RBS_1775</t>
+  </si>
+  <si>
+    <t>RBS_1992</t>
+  </si>
+  <si>
+    <t>RBS_2064</t>
+  </si>
+  <si>
+    <t>RBS_1412</t>
+  </si>
+  <si>
+    <t>RBS_2866</t>
+  </si>
+  <si>
+    <t>RBS_2604</t>
+  </si>
+  <si>
+    <t>RBS_2005</t>
+  </si>
+  <si>
+    <t>RBS_1743</t>
+  </si>
+  <si>
+    <t>RBS_330</t>
+  </si>
+  <si>
+    <t>RBS_1888</t>
+  </si>
+  <si>
+    <t>RBS_3029</t>
+  </si>
+  <si>
+    <t>RBS_1383</t>
+  </si>
+  <si>
+    <t>RBS_1349</t>
+  </si>
+  <si>
+    <t>RBS_2992</t>
+  </si>
+  <si>
+    <t>RBS_391</t>
+  </si>
+  <si>
+    <t>RBS_1124</t>
+  </si>
+  <si>
+    <t>RBS_2540</t>
+  </si>
+  <si>
+    <t>RBS_2122</t>
+  </si>
+  <si>
+    <t>RBS_1297</t>
+  </si>
+  <si>
+    <t>RBS_3718</t>
+  </si>
+  <si>
+    <t>RBS_3231</t>
+  </si>
+  <si>
+    <t>RBS_1343</t>
+  </si>
+  <si>
+    <t>RBS_2437</t>
+  </si>
+  <si>
+    <t>RBS_1782</t>
+  </si>
+  <si>
+    <t>RBS_1371</t>
+  </si>
+  <si>
+    <t>RBS_3041</t>
+  </si>
+  <si>
+    <t>RBS_1999</t>
+  </si>
+  <si>
+    <t>RBS_1360</t>
+  </si>
+  <si>
+    <t>RBS_2014</t>
+  </si>
+  <si>
+    <t>RBS_2610</t>
+  </si>
+  <si>
+    <t>RBS_1351</t>
+  </si>
+  <si>
+    <t>RBS_3692</t>
+  </si>
+  <si>
+    <t>RBS_3045</t>
+  </si>
+  <si>
+    <t>RBS_3112</t>
+  </si>
+  <si>
+    <t>RBS_1416</t>
+  </si>
+  <si>
+    <t>RBS_2027</t>
+  </si>
+  <si>
+    <t>RBS_2431</t>
+  </si>
+  <si>
+    <t>RBS_2140</t>
+  </si>
+  <si>
+    <t>RBS_1112</t>
+  </si>
+  <si>
+    <t>RBS_2856</t>
+  </si>
+  <si>
+    <t>RBS_1294</t>
+  </si>
+  <si>
+    <t>RBS_2998</t>
+  </si>
+  <si>
+    <t>RBS_1400</t>
+  </si>
+  <si>
+    <t>RBS_2652</t>
+  </si>
+  <si>
+    <t>Fourth_Plate</t>
+  </si>
+  <si>
+    <t>TTTAAGACAGGCTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGCGCTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGTGGCTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACAGGAGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGGGCTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGCAGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACATGCTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACAGGTTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGCATTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACACGCTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACAGAGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGTTGCTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGCGTTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACCGAGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGCACTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGTGGAGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGATTGGCTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACCTAGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGGGTTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGTGCTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGCCAGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGATAGGAGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACATAGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACAGCTATATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGCCGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGATAGGCTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACCTGCTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGCTCTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGATACGCTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGTGGTTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACACGAGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACAGCGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACATACTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGTTGAGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGATTGGAGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGACGCTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGCGAGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACCTATTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGATCGAGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACATGAGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGATAGAGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGGGAGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACACGTTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGCGGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACAGCTTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGCCTATATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGTGCGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACAGACTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACACGGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGTGAGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACTTGCTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACCTACTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACAGGCATATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGTGAGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAAGGGCTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGTTGTTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGATACAGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGCCTTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGCATATATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGATAGGTTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAAGCGCTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGACGAGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACCCAGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACATATTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGGGCATATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGATTGGTTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGATGGGCTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGCAGCTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACCAGCTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGTGCTATATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGCCATTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGATACGAGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACAGGACTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGCGCATATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACAGCAGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACCTGAGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGCATCTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGATTGAGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGATACGGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGATATGCTTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGTGGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACAGCTCTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACCAGGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACATCAGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGACAGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACTTGAGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGGGGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGATAGCGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGAGGTAGGTATACAT</t>
+  </si>
+  <si>
+    <t>TTTAAGACCTTCTTATACAT</t>
+  </si>
+  <si>
+    <t>CAGGCT</t>
+  </si>
+  <si>
+    <t>GGCGCT</t>
+  </si>
+  <si>
+    <t>GTGGCT</t>
+  </si>
+  <si>
+    <t>CAGGAG</t>
+  </si>
+  <si>
+    <t>GGGGCT</t>
+  </si>
+  <si>
+    <t>GGCAGG</t>
+  </si>
+  <si>
+    <t>CATGCT</t>
+  </si>
+  <si>
+    <t>CAGGTT</t>
+  </si>
+  <si>
+    <t>GGCATT</t>
+  </si>
+  <si>
+    <t>CACGCT</t>
+  </si>
+  <si>
+    <t>CAGAGG</t>
+  </si>
+  <si>
+    <t>GTTGCT</t>
+  </si>
+  <si>
+    <t>GGCGTT</t>
+  </si>
+  <si>
+    <t>CCGAGG</t>
+  </si>
+  <si>
+    <t>GGCACT</t>
+  </si>
+  <si>
+    <t>GTGGAG</t>
+  </si>
+  <si>
+    <t>TTGGCT</t>
+  </si>
+  <si>
+    <t>CCTAGG</t>
+  </si>
+  <si>
+    <t>GGGGTT</t>
+  </si>
+  <si>
+    <t>GGTGCT</t>
+  </si>
+  <si>
+    <t>GGCCAG</t>
+  </si>
+  <si>
+    <t>TAGGAG</t>
+  </si>
+  <si>
+    <t>CATAGG</t>
+  </si>
+  <si>
+    <t>CAGCTA</t>
+  </si>
+  <si>
+    <t>GGCCGG</t>
+  </si>
+  <si>
+    <t>TAGGCT</t>
+  </si>
+  <si>
+    <t>CCTGCT</t>
+  </si>
+  <si>
+    <t>GGCTCT</t>
+  </si>
+  <si>
+    <t>TACGCT</t>
+  </si>
+  <si>
+    <t>GTGGTT</t>
+  </si>
+  <si>
+    <t>CACGAG</t>
+  </si>
+  <si>
+    <t>CAGCGG</t>
+  </si>
+  <si>
+    <t>CATACT</t>
+  </si>
+  <si>
+    <t>GTTGAG</t>
+  </si>
+  <si>
+    <t>TTGGAG</t>
+  </si>
+  <si>
+    <t>GACGCT</t>
+  </si>
+  <si>
+    <t>GGCGAG</t>
+  </si>
+  <si>
+    <t>CCTATT</t>
+  </si>
+  <si>
+    <t>TCGAGG</t>
+  </si>
+  <si>
+    <t>CATGAG</t>
+  </si>
+  <si>
+    <t>TAGAGG</t>
+  </si>
+  <si>
+    <t>GGGGAG</t>
+  </si>
+  <si>
+    <t>CACGTT</t>
+  </si>
+  <si>
+    <t>GGCGGG</t>
+  </si>
+  <si>
+    <t>CAGCTT</t>
+  </si>
+  <si>
+    <t>GGCCTA</t>
+  </si>
+  <si>
+    <t>GTGCGG</t>
+  </si>
+  <si>
+    <t>CAGACT</t>
+  </si>
+  <si>
+    <t>CACGGG</t>
+  </si>
+  <si>
+    <t>GGTGAG</t>
+  </si>
+  <si>
+    <t>CTTGCT</t>
+  </si>
+  <si>
+    <t>CCTACT</t>
+  </si>
+  <si>
+    <t>CAGGCA</t>
+  </si>
+  <si>
+    <t>GTGAGG</t>
+  </si>
+  <si>
+    <t>AGGGCT</t>
+  </si>
+  <si>
+    <t>GTTGTT</t>
+  </si>
+  <si>
+    <t>TACAGG</t>
+  </si>
+  <si>
+    <t>GGCCTT</t>
+  </si>
+  <si>
+    <t>GGCATA</t>
+  </si>
+  <si>
+    <t>TAGGTT</t>
+  </si>
+  <si>
+    <t>AGCGCT</t>
+  </si>
+  <si>
+    <t>GACGAG</t>
+  </si>
+  <si>
+    <t>CCCAGG</t>
+  </si>
+  <si>
+    <t>CATATT</t>
+  </si>
+  <si>
+    <t>GGGGCA</t>
+  </si>
+  <si>
+    <t>TTGGTT</t>
+  </si>
+  <si>
+    <t>TGGGCT</t>
+  </si>
+  <si>
+    <t>GGCAGC</t>
+  </si>
+  <si>
+    <t>CCAGCT</t>
+  </si>
+  <si>
+    <t>GTGCTA</t>
+  </si>
+  <si>
+    <t>GGCCAT</t>
+  </si>
+  <si>
+    <t>TACGAG</t>
+  </si>
+  <si>
+    <t>CAGGAC</t>
+  </si>
+  <si>
+    <t>GGCGCA</t>
+  </si>
+  <si>
+    <t>CAGCAG</t>
+  </si>
+  <si>
+    <t>CCTGAG</t>
+  </si>
+  <si>
+    <t>GGCATC</t>
+  </si>
+  <si>
+    <t>TTGAGG</t>
+  </si>
+  <si>
+    <t>TACGGG</t>
+  </si>
+  <si>
+    <t>TATGCT</t>
+  </si>
+  <si>
+    <t>GGTGGG</t>
+  </si>
+  <si>
+    <t>CAGCTC</t>
+  </si>
+  <si>
+    <t>CCAGGG</t>
+  </si>
+  <si>
+    <t>CATCAG</t>
+  </si>
+  <si>
+    <t>GACAGG</t>
+  </si>
+  <si>
+    <t>CTTGAG</t>
+  </si>
+  <si>
+    <t>GGGGGG</t>
+  </si>
+  <si>
+    <t>TAGCGG</t>
+  </si>
+  <si>
+    <t>GGTAGG</t>
+  </si>
+  <si>
+    <t>CCTTCT</t>
   </si>
 </sst>
 </file>
@@ -2253,12 +3066,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2576,10 +3392,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F269"/>
+  <dimension ref="A1:F359"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A249" workbookViewId="0">
-      <selection activeCell="H266" sqref="H266"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -8147,6 +8963,1806 @@
         <v>1</v>
       </c>
     </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A270" s="5" t="s">
+        <v>725</v>
+      </c>
+      <c r="B270" s="6" t="s">
+        <v>816</v>
+      </c>
+      <c r="C270" s="7" t="s">
+        <v>906</v>
+      </c>
+      <c r="D270" t="s">
+        <v>815</v>
+      </c>
+      <c r="E270" t="s">
+        <v>128</v>
+      </c>
+      <c r="F270">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A271" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="B271" s="6" t="s">
+        <v>817</v>
+      </c>
+      <c r="C271" s="7" t="s">
+        <v>907</v>
+      </c>
+      <c r="D271" t="s">
+        <v>815</v>
+      </c>
+      <c r="E271" t="s">
+        <v>131</v>
+      </c>
+      <c r="F271">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A272" s="5" t="s">
+        <v>727</v>
+      </c>
+      <c r="B272" s="6" t="s">
+        <v>818</v>
+      </c>
+      <c r="C272" s="7" t="s">
+        <v>908</v>
+      </c>
+      <c r="D272" t="s">
+        <v>815</v>
+      </c>
+      <c r="E272" t="s">
+        <v>132</v>
+      </c>
+      <c r="F272">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A273" s="5" t="s">
+        <v>728</v>
+      </c>
+      <c r="B273" s="6" t="s">
+        <v>819</v>
+      </c>
+      <c r="C273" s="7" t="s">
+        <v>909</v>
+      </c>
+      <c r="D273" t="s">
+        <v>815</v>
+      </c>
+      <c r="E273" t="s">
+        <v>133</v>
+      </c>
+      <c r="F273">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A274" s="5" t="s">
+        <v>729</v>
+      </c>
+      <c r="B274" s="6" t="s">
+        <v>820</v>
+      </c>
+      <c r="C274" s="7" t="s">
+        <v>910</v>
+      </c>
+      <c r="D274" t="s">
+        <v>815</v>
+      </c>
+      <c r="E274" t="s">
+        <v>134</v>
+      </c>
+      <c r="F274">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A275" s="5" t="s">
+        <v>730</v>
+      </c>
+      <c r="B275" s="6" t="s">
+        <v>821</v>
+      </c>
+      <c r="C275" s="7" t="s">
+        <v>911</v>
+      </c>
+      <c r="D275" t="s">
+        <v>815</v>
+      </c>
+      <c r="E275" t="s">
+        <v>135</v>
+      </c>
+      <c r="F275">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A276" s="5" t="s">
+        <v>731</v>
+      </c>
+      <c r="B276" s="6" t="s">
+        <v>822</v>
+      </c>
+      <c r="C276" s="7" t="s">
+        <v>912</v>
+      </c>
+      <c r="D276" t="s">
+        <v>815</v>
+      </c>
+      <c r="E276" t="s">
+        <v>136</v>
+      </c>
+      <c r="F276">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A277" s="5" t="s">
+        <v>732</v>
+      </c>
+      <c r="B277" s="6" t="s">
+        <v>823</v>
+      </c>
+      <c r="C277" s="7" t="s">
+        <v>913</v>
+      </c>
+      <c r="D277" t="s">
+        <v>815</v>
+      </c>
+      <c r="E277" t="s">
+        <v>137</v>
+      </c>
+      <c r="F277">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A278" s="5" t="s">
+        <v>733</v>
+      </c>
+      <c r="B278" s="6" t="s">
+        <v>824</v>
+      </c>
+      <c r="C278" s="7" t="s">
+        <v>914</v>
+      </c>
+      <c r="D278" t="s">
+        <v>815</v>
+      </c>
+      <c r="E278" t="s">
+        <v>138</v>
+      </c>
+      <c r="F278">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A279" s="5" t="s">
+        <v>734</v>
+      </c>
+      <c r="B279" s="6" t="s">
+        <v>825</v>
+      </c>
+      <c r="C279" s="7" t="s">
+        <v>915</v>
+      </c>
+      <c r="D279" t="s">
+        <v>815</v>
+      </c>
+      <c r="E279" t="s">
+        <v>139</v>
+      </c>
+      <c r="F279">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A280" s="5" t="s">
+        <v>735</v>
+      </c>
+      <c r="B280" s="6" t="s">
+        <v>826</v>
+      </c>
+      <c r="C280" s="7" t="s">
+        <v>916</v>
+      </c>
+      <c r="D280" t="s">
+        <v>815</v>
+      </c>
+      <c r="E280" t="s">
+        <v>140</v>
+      </c>
+      <c r="F280">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A281" s="5" t="s">
+        <v>736</v>
+      </c>
+      <c r="B281" s="6" t="s">
+        <v>827</v>
+      </c>
+      <c r="C281" s="7" t="s">
+        <v>917</v>
+      </c>
+      <c r="D281" t="s">
+        <v>815</v>
+      </c>
+      <c r="E281" t="s">
+        <v>141</v>
+      </c>
+      <c r="F281">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A282" s="5" t="s">
+        <v>737</v>
+      </c>
+      <c r="B282" s="6" t="s">
+        <v>828</v>
+      </c>
+      <c r="C282" s="7" t="s">
+        <v>918</v>
+      </c>
+      <c r="D282" t="s">
+        <v>815</v>
+      </c>
+      <c r="E282" t="s">
+        <v>142</v>
+      </c>
+      <c r="F282">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A283" s="5" t="s">
+        <v>738</v>
+      </c>
+      <c r="B283" s="6" t="s">
+        <v>829</v>
+      </c>
+      <c r="C283" s="7" t="s">
+        <v>919</v>
+      </c>
+      <c r="D283" t="s">
+        <v>815</v>
+      </c>
+      <c r="E283" t="s">
+        <v>143</v>
+      </c>
+      <c r="F283">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A284" s="5" t="s">
+        <v>739</v>
+      </c>
+      <c r="B284" s="6" t="s">
+        <v>830</v>
+      </c>
+      <c r="C284" s="7" t="s">
+        <v>920</v>
+      </c>
+      <c r="D284" t="s">
+        <v>815</v>
+      </c>
+      <c r="E284" t="s">
+        <v>144</v>
+      </c>
+      <c r="F284">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A285" s="5" t="s">
+        <v>740</v>
+      </c>
+      <c r="B285" s="6" t="s">
+        <v>831</v>
+      </c>
+      <c r="C285" s="7" t="s">
+        <v>921</v>
+      </c>
+      <c r="D285" t="s">
+        <v>815</v>
+      </c>
+      <c r="E285" t="s">
+        <v>145</v>
+      </c>
+      <c r="F285">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A286" s="5" t="s">
+        <v>741</v>
+      </c>
+      <c r="B286" s="6" t="s">
+        <v>832</v>
+      </c>
+      <c r="C286" s="7" t="s">
+        <v>922</v>
+      </c>
+      <c r="D286" t="s">
+        <v>815</v>
+      </c>
+      <c r="E286" t="s">
+        <v>146</v>
+      </c>
+      <c r="F286">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A287" s="5" t="s">
+        <v>742</v>
+      </c>
+      <c r="B287" s="6" t="s">
+        <v>833</v>
+      </c>
+      <c r="C287" s="7" t="s">
+        <v>923</v>
+      </c>
+      <c r="D287" t="s">
+        <v>815</v>
+      </c>
+      <c r="E287" t="s">
+        <v>147</v>
+      </c>
+      <c r="F287">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A288" s="5" t="s">
+        <v>743</v>
+      </c>
+      <c r="B288" s="6" t="s">
+        <v>834</v>
+      </c>
+      <c r="C288" s="7" t="s">
+        <v>924</v>
+      </c>
+      <c r="D288" t="s">
+        <v>815</v>
+      </c>
+      <c r="E288" t="s">
+        <v>148</v>
+      </c>
+      <c r="F288">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A289" s="5" t="s">
+        <v>744</v>
+      </c>
+      <c r="B289" s="6" t="s">
+        <v>835</v>
+      </c>
+      <c r="C289" s="7" t="s">
+        <v>925</v>
+      </c>
+      <c r="D289" t="s">
+        <v>815</v>
+      </c>
+      <c r="E289" t="s">
+        <v>149</v>
+      </c>
+      <c r="F289">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A290" s="5" t="s">
+        <v>745</v>
+      </c>
+      <c r="B290" s="6" t="s">
+        <v>836</v>
+      </c>
+      <c r="C290" s="7" t="s">
+        <v>926</v>
+      </c>
+      <c r="D290" t="s">
+        <v>815</v>
+      </c>
+      <c r="E290" t="s">
+        <v>150</v>
+      </c>
+      <c r="F290">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A291" s="5" t="s">
+        <v>746</v>
+      </c>
+      <c r="B291" s="6" t="s">
+        <v>837</v>
+      </c>
+      <c r="C291" s="7" t="s">
+        <v>927</v>
+      </c>
+      <c r="D291" t="s">
+        <v>815</v>
+      </c>
+      <c r="E291" t="s">
+        <v>151</v>
+      </c>
+      <c r="F291">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A292" s="5" t="s">
+        <v>747</v>
+      </c>
+      <c r="B292" s="6" t="s">
+        <v>838</v>
+      </c>
+      <c r="C292" s="7" t="s">
+        <v>928</v>
+      </c>
+      <c r="D292" t="s">
+        <v>815</v>
+      </c>
+      <c r="E292" t="s">
+        <v>152</v>
+      </c>
+      <c r="F292">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A293" s="5" t="s">
+        <v>748</v>
+      </c>
+      <c r="B293" s="6" t="s">
+        <v>839</v>
+      </c>
+      <c r="C293" s="7" t="s">
+        <v>929</v>
+      </c>
+      <c r="D293" t="s">
+        <v>815</v>
+      </c>
+      <c r="E293" t="s">
+        <v>153</v>
+      </c>
+      <c r="F293">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A294" s="5" t="s">
+        <v>749</v>
+      </c>
+      <c r="B294" s="6" t="s">
+        <v>840</v>
+      </c>
+      <c r="C294" s="7" t="s">
+        <v>930</v>
+      </c>
+      <c r="D294" t="s">
+        <v>815</v>
+      </c>
+      <c r="E294" t="s">
+        <v>129</v>
+      </c>
+      <c r="F294">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A295" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="B295" s="6" t="s">
+        <v>841</v>
+      </c>
+      <c r="C295" s="7" t="s">
+        <v>931</v>
+      </c>
+      <c r="D295" t="s">
+        <v>815</v>
+      </c>
+      <c r="E295" t="s">
+        <v>154</v>
+      </c>
+      <c r="F295">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A296" s="5" t="s">
+        <v>751</v>
+      </c>
+      <c r="B296" s="6" t="s">
+        <v>842</v>
+      </c>
+      <c r="C296" s="7" t="s">
+        <v>932</v>
+      </c>
+      <c r="D296" t="s">
+        <v>815</v>
+      </c>
+      <c r="E296" t="s">
+        <v>155</v>
+      </c>
+      <c r="F296">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A297" s="5" t="s">
+        <v>752</v>
+      </c>
+      <c r="B297" s="6" t="s">
+        <v>843</v>
+      </c>
+      <c r="C297" s="7" t="s">
+        <v>933</v>
+      </c>
+      <c r="D297" t="s">
+        <v>815</v>
+      </c>
+      <c r="E297" t="s">
+        <v>156</v>
+      </c>
+      <c r="F297">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A298" s="5" t="s">
+        <v>753</v>
+      </c>
+      <c r="B298" s="6" t="s">
+        <v>844</v>
+      </c>
+      <c r="C298" s="7" t="s">
+        <v>934</v>
+      </c>
+      <c r="D298" t="s">
+        <v>815</v>
+      </c>
+      <c r="E298" t="s">
+        <v>157</v>
+      </c>
+      <c r="F298">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A299" s="5" t="s">
+        <v>754</v>
+      </c>
+      <c r="B299" s="6" t="s">
+        <v>845</v>
+      </c>
+      <c r="C299" s="7" t="s">
+        <v>935</v>
+      </c>
+      <c r="D299" t="s">
+        <v>815</v>
+      </c>
+      <c r="E299" t="s">
+        <v>158</v>
+      </c>
+      <c r="F299">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A300" s="5" t="s">
+        <v>755</v>
+      </c>
+      <c r="B300" s="6" t="s">
+        <v>846</v>
+      </c>
+      <c r="C300" s="7" t="s">
+        <v>936</v>
+      </c>
+      <c r="D300" t="s">
+        <v>815</v>
+      </c>
+      <c r="E300" t="s">
+        <v>159</v>
+      </c>
+      <c r="F300">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A301" s="5" t="s">
+        <v>756</v>
+      </c>
+      <c r="B301" s="6" t="s">
+        <v>847</v>
+      </c>
+      <c r="C301" s="7" t="s">
+        <v>937</v>
+      </c>
+      <c r="D301" t="s">
+        <v>815</v>
+      </c>
+      <c r="E301" t="s">
+        <v>160</v>
+      </c>
+      <c r="F301">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A302" s="5" t="s">
+        <v>757</v>
+      </c>
+      <c r="B302" s="6" t="s">
+        <v>848</v>
+      </c>
+      <c r="C302" s="7" t="s">
+        <v>938</v>
+      </c>
+      <c r="D302" t="s">
+        <v>815</v>
+      </c>
+      <c r="E302" t="s">
+        <v>161</v>
+      </c>
+      <c r="F302">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A303" s="5" t="s">
+        <v>758</v>
+      </c>
+      <c r="B303" s="6" t="s">
+        <v>849</v>
+      </c>
+      <c r="C303" s="7" t="s">
+        <v>939</v>
+      </c>
+      <c r="D303" t="s">
+        <v>815</v>
+      </c>
+      <c r="E303" t="s">
+        <v>162</v>
+      </c>
+      <c r="F303">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A304" s="5" t="s">
+        <v>759</v>
+      </c>
+      <c r="B304" s="6" t="s">
+        <v>850</v>
+      </c>
+      <c r="C304" s="7" t="s">
+        <v>940</v>
+      </c>
+      <c r="D304" t="s">
+        <v>815</v>
+      </c>
+      <c r="E304" t="s">
+        <v>163</v>
+      </c>
+      <c r="F304">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A305" s="5" t="s">
+        <v>760</v>
+      </c>
+      <c r="B305" s="6" t="s">
+        <v>851</v>
+      </c>
+      <c r="C305" s="7" t="s">
+        <v>941</v>
+      </c>
+      <c r="D305" t="s">
+        <v>815</v>
+      </c>
+      <c r="E305" t="s">
+        <v>164</v>
+      </c>
+      <c r="F305">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A306" s="5" t="s">
+        <v>761</v>
+      </c>
+      <c r="B306" s="6" t="s">
+        <v>852</v>
+      </c>
+      <c r="C306" s="7" t="s">
+        <v>942</v>
+      </c>
+      <c r="D306" t="s">
+        <v>815</v>
+      </c>
+      <c r="E306" t="s">
+        <v>165</v>
+      </c>
+      <c r="F306">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A307" s="5" t="s">
+        <v>762</v>
+      </c>
+      <c r="B307" s="6" t="s">
+        <v>853</v>
+      </c>
+      <c r="C307" s="7" t="s">
+        <v>943</v>
+      </c>
+      <c r="D307" t="s">
+        <v>815</v>
+      </c>
+      <c r="E307" t="s">
+        <v>166</v>
+      </c>
+      <c r="F307">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A308" s="5" t="s">
+        <v>763</v>
+      </c>
+      <c r="B308" s="6" t="s">
+        <v>854</v>
+      </c>
+      <c r="C308" s="7" t="s">
+        <v>944</v>
+      </c>
+      <c r="D308" t="s">
+        <v>815</v>
+      </c>
+      <c r="E308" t="s">
+        <v>167</v>
+      </c>
+      <c r="F308">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A309" s="5" t="s">
+        <v>764</v>
+      </c>
+      <c r="B309" s="6" t="s">
+        <v>855</v>
+      </c>
+      <c r="C309" s="7" t="s">
+        <v>945</v>
+      </c>
+      <c r="D309" t="s">
+        <v>815</v>
+      </c>
+      <c r="E309" t="s">
+        <v>168</v>
+      </c>
+      <c r="F309">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A310" s="5" t="s">
+        <v>765</v>
+      </c>
+      <c r="B310" s="6" t="s">
+        <v>856</v>
+      </c>
+      <c r="C310" s="7" t="s">
+        <v>946</v>
+      </c>
+      <c r="D310" t="s">
+        <v>815</v>
+      </c>
+      <c r="E310" t="s">
+        <v>169</v>
+      </c>
+      <c r="F310">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A311" s="5" t="s">
+        <v>766</v>
+      </c>
+      <c r="B311" s="6" t="s">
+        <v>857</v>
+      </c>
+      <c r="C311" s="7" t="s">
+        <v>947</v>
+      </c>
+      <c r="D311" t="s">
+        <v>815</v>
+      </c>
+      <c r="E311" t="s">
+        <v>170</v>
+      </c>
+      <c r="F311">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A312" s="5" t="s">
+        <v>767</v>
+      </c>
+      <c r="B312" s="6" t="s">
+        <v>858</v>
+      </c>
+      <c r="C312" s="7" t="s">
+        <v>948</v>
+      </c>
+      <c r="D312" t="s">
+        <v>815</v>
+      </c>
+      <c r="E312" t="s">
+        <v>171</v>
+      </c>
+      <c r="F312">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A313" s="5" t="s">
+        <v>768</v>
+      </c>
+      <c r="B313" s="6" t="s">
+        <v>859</v>
+      </c>
+      <c r="C313" s="7" t="s">
+        <v>949</v>
+      </c>
+      <c r="D313" t="s">
+        <v>815</v>
+      </c>
+      <c r="E313" t="s">
+        <v>172</v>
+      </c>
+      <c r="F313">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A314" s="5" t="s">
+        <v>769</v>
+      </c>
+      <c r="B314" s="6" t="s">
+        <v>860</v>
+      </c>
+      <c r="C314" s="7" t="s">
+        <v>950</v>
+      </c>
+      <c r="D314" t="s">
+        <v>815</v>
+      </c>
+      <c r="E314" t="s">
+        <v>173</v>
+      </c>
+      <c r="F314">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A315" s="5" t="s">
+        <v>770</v>
+      </c>
+      <c r="B315" s="6" t="s">
+        <v>861</v>
+      </c>
+      <c r="C315" s="7" t="s">
+        <v>951</v>
+      </c>
+      <c r="D315" t="s">
+        <v>815</v>
+      </c>
+      <c r="E315" t="s">
+        <v>174</v>
+      </c>
+      <c r="F315">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A316" s="5" t="s">
+        <v>771</v>
+      </c>
+      <c r="B316" s="6" t="s">
+        <v>862</v>
+      </c>
+      <c r="C316" s="7" t="s">
+        <v>952</v>
+      </c>
+      <c r="D316" t="s">
+        <v>815</v>
+      </c>
+      <c r="E316" t="s">
+        <v>175</v>
+      </c>
+      <c r="F316">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A317" s="5" t="s">
+        <v>772</v>
+      </c>
+      <c r="B317" s="6" t="s">
+        <v>863</v>
+      </c>
+      <c r="C317" s="7" t="s">
+        <v>953</v>
+      </c>
+      <c r="D317" t="s">
+        <v>815</v>
+      </c>
+      <c r="E317" t="s">
+        <v>176</v>
+      </c>
+      <c r="F317">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A318" s="5" t="s">
+        <v>773</v>
+      </c>
+      <c r="B318" s="6" t="s">
+        <v>864</v>
+      </c>
+      <c r="C318" s="7" t="s">
+        <v>954</v>
+      </c>
+      <c r="D318" t="s">
+        <v>815</v>
+      </c>
+      <c r="E318" t="s">
+        <v>177</v>
+      </c>
+      <c r="F318">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A319" s="5" t="s">
+        <v>774</v>
+      </c>
+      <c r="B319" s="6" t="s">
+        <v>865</v>
+      </c>
+      <c r="C319" s="7" t="s">
+        <v>955</v>
+      </c>
+      <c r="D319" t="s">
+        <v>815</v>
+      </c>
+      <c r="E319" t="s">
+        <v>178</v>
+      </c>
+      <c r="F319">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A320" s="5" t="s">
+        <v>775</v>
+      </c>
+      <c r="B320" s="6" t="s">
+        <v>866</v>
+      </c>
+      <c r="C320" s="7" t="s">
+        <v>956</v>
+      </c>
+      <c r="D320" t="s">
+        <v>815</v>
+      </c>
+      <c r="E320" t="s">
+        <v>179</v>
+      </c>
+      <c r="F320">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A321" s="5" t="s">
+        <v>776</v>
+      </c>
+      <c r="B321" s="6" t="s">
+        <v>867</v>
+      </c>
+      <c r="C321" s="7" t="s">
+        <v>957</v>
+      </c>
+      <c r="D321" t="s">
+        <v>815</v>
+      </c>
+      <c r="E321" t="s">
+        <v>180</v>
+      </c>
+      <c r="F321">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A322" s="5" t="s">
+        <v>777</v>
+      </c>
+      <c r="B322" s="6" t="s">
+        <v>868</v>
+      </c>
+      <c r="C322" s="7" t="s">
+        <v>958</v>
+      </c>
+      <c r="D322" t="s">
+        <v>815</v>
+      </c>
+      <c r="E322" t="s">
+        <v>181</v>
+      </c>
+      <c r="F322">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A323" s="5" t="s">
+        <v>778</v>
+      </c>
+      <c r="B323" s="6" t="s">
+        <v>869</v>
+      </c>
+      <c r="C323" s="7" t="s">
+        <v>959</v>
+      </c>
+      <c r="D323" t="s">
+        <v>815</v>
+      </c>
+      <c r="E323" t="s">
+        <v>182</v>
+      </c>
+      <c r="F323">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A324" s="5" t="s">
+        <v>779</v>
+      </c>
+      <c r="B324" s="6" t="s">
+        <v>870</v>
+      </c>
+      <c r="C324" s="7" t="s">
+        <v>960</v>
+      </c>
+      <c r="D324" t="s">
+        <v>815</v>
+      </c>
+      <c r="E324" t="s">
+        <v>183</v>
+      </c>
+      <c r="F324">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A325" s="5" t="s">
+        <v>780</v>
+      </c>
+      <c r="B325" s="6" t="s">
+        <v>871</v>
+      </c>
+      <c r="C325" s="7" t="s">
+        <v>961</v>
+      </c>
+      <c r="D325" t="s">
+        <v>815</v>
+      </c>
+      <c r="E325" t="s">
+        <v>184</v>
+      </c>
+      <c r="F325">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A326" s="5" t="s">
+        <v>781</v>
+      </c>
+      <c r="B326" s="6" t="s">
+        <v>872</v>
+      </c>
+      <c r="C326" s="7" t="s">
+        <v>962</v>
+      </c>
+      <c r="D326" t="s">
+        <v>815</v>
+      </c>
+      <c r="E326" t="s">
+        <v>185</v>
+      </c>
+      <c r="F326">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A327" s="5" t="s">
+        <v>782</v>
+      </c>
+      <c r="B327" s="6" t="s">
+        <v>873</v>
+      </c>
+      <c r="C327" s="7" t="s">
+        <v>963</v>
+      </c>
+      <c r="D327" t="s">
+        <v>815</v>
+      </c>
+      <c r="E327" t="s">
+        <v>186</v>
+      </c>
+      <c r="F327">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A328" s="5" t="s">
+        <v>783</v>
+      </c>
+      <c r="B328" s="6" t="s">
+        <v>874</v>
+      </c>
+      <c r="C328" s="7" t="s">
+        <v>964</v>
+      </c>
+      <c r="D328" t="s">
+        <v>815</v>
+      </c>
+      <c r="E328" t="s">
+        <v>187</v>
+      </c>
+      <c r="F328">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A329" s="5" t="s">
+        <v>784</v>
+      </c>
+      <c r="B329" s="6" t="s">
+        <v>875</v>
+      </c>
+      <c r="C329" s="7" t="s">
+        <v>965</v>
+      </c>
+      <c r="D329" t="s">
+        <v>815</v>
+      </c>
+      <c r="E329" t="s">
+        <v>188</v>
+      </c>
+      <c r="F329">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A330" s="5" t="s">
+        <v>785</v>
+      </c>
+      <c r="B330" s="6" t="s">
+        <v>876</v>
+      </c>
+      <c r="C330" s="7" t="s">
+        <v>966</v>
+      </c>
+      <c r="D330" t="s">
+        <v>815</v>
+      </c>
+      <c r="E330" t="s">
+        <v>189</v>
+      </c>
+      <c r="F330">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A331" s="5" t="s">
+        <v>786</v>
+      </c>
+      <c r="B331" s="6" t="s">
+        <v>877</v>
+      </c>
+      <c r="C331" s="7" t="s">
+        <v>967</v>
+      </c>
+      <c r="D331" t="s">
+        <v>815</v>
+      </c>
+      <c r="E331" t="s">
+        <v>190</v>
+      </c>
+      <c r="F331">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A332" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="B332" s="6" t="s">
+        <v>878</v>
+      </c>
+      <c r="C332" s="7" t="s">
+        <v>968</v>
+      </c>
+      <c r="D332" t="s">
+        <v>815</v>
+      </c>
+      <c r="E332" t="s">
+        <v>191</v>
+      </c>
+      <c r="F332">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A333" s="5" t="s">
+        <v>788</v>
+      </c>
+      <c r="B333" s="6" t="s">
+        <v>879</v>
+      </c>
+      <c r="C333" s="7" t="s">
+        <v>969</v>
+      </c>
+      <c r="D333" t="s">
+        <v>815</v>
+      </c>
+      <c r="E333" t="s">
+        <v>192</v>
+      </c>
+      <c r="F333">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A334" s="5" t="s">
+        <v>789</v>
+      </c>
+      <c r="B334" s="6" t="s">
+        <v>880</v>
+      </c>
+      <c r="C334" s="7" t="s">
+        <v>970</v>
+      </c>
+      <c r="D334" t="s">
+        <v>815</v>
+      </c>
+      <c r="E334" t="s">
+        <v>193</v>
+      </c>
+      <c r="F334">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A335" s="5" t="s">
+        <v>790</v>
+      </c>
+      <c r="B335" s="6" t="s">
+        <v>881</v>
+      </c>
+      <c r="C335" s="7" t="s">
+        <v>971</v>
+      </c>
+      <c r="D335" t="s">
+        <v>815</v>
+      </c>
+      <c r="E335" t="s">
+        <v>194</v>
+      </c>
+      <c r="F335">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A336" s="5" t="s">
+        <v>791</v>
+      </c>
+      <c r="B336" s="6" t="s">
+        <v>882</v>
+      </c>
+      <c r="C336" s="7" t="s">
+        <v>972</v>
+      </c>
+      <c r="D336" t="s">
+        <v>815</v>
+      </c>
+      <c r="E336" t="s">
+        <v>195</v>
+      </c>
+      <c r="F336">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A337" s="5" t="s">
+        <v>792</v>
+      </c>
+      <c r="B337" s="6" t="s">
+        <v>883</v>
+      </c>
+      <c r="C337" s="7" t="s">
+        <v>973</v>
+      </c>
+      <c r="D337" t="s">
+        <v>815</v>
+      </c>
+      <c r="E337" t="s">
+        <v>196</v>
+      </c>
+      <c r="F337">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A338" s="5" t="s">
+        <v>793</v>
+      </c>
+      <c r="B338" s="6" t="s">
+        <v>884</v>
+      </c>
+      <c r="C338" s="7" t="s">
+        <v>974</v>
+      </c>
+      <c r="D338" t="s">
+        <v>815</v>
+      </c>
+      <c r="E338" t="s">
+        <v>197</v>
+      </c>
+      <c r="F338">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A339" s="5" t="s">
+        <v>794</v>
+      </c>
+      <c r="B339" s="6" t="s">
+        <v>885</v>
+      </c>
+      <c r="C339" s="7" t="s">
+        <v>975</v>
+      </c>
+      <c r="D339" t="s">
+        <v>815</v>
+      </c>
+      <c r="E339" t="s">
+        <v>198</v>
+      </c>
+      <c r="F339">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A340" s="5" t="s">
+        <v>795</v>
+      </c>
+      <c r="B340" s="6" t="s">
+        <v>886</v>
+      </c>
+      <c r="C340" s="7" t="s">
+        <v>976</v>
+      </c>
+      <c r="D340" t="s">
+        <v>815</v>
+      </c>
+      <c r="E340" t="s">
+        <v>199</v>
+      </c>
+      <c r="F340">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A341" s="5" t="s">
+        <v>796</v>
+      </c>
+      <c r="B341" s="6" t="s">
+        <v>887</v>
+      </c>
+      <c r="C341" s="7" t="s">
+        <v>977</v>
+      </c>
+      <c r="D341" t="s">
+        <v>815</v>
+      </c>
+      <c r="E341" t="s">
+        <v>200</v>
+      </c>
+      <c r="F341">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A342" s="5" t="s">
+        <v>797</v>
+      </c>
+      <c r="B342" s="6" t="s">
+        <v>888</v>
+      </c>
+      <c r="C342" s="7" t="s">
+        <v>978</v>
+      </c>
+      <c r="D342" t="s">
+        <v>815</v>
+      </c>
+      <c r="E342" t="s">
+        <v>130</v>
+      </c>
+      <c r="F342">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A343" s="5" t="s">
+        <v>798</v>
+      </c>
+      <c r="B343" s="6" t="s">
+        <v>889</v>
+      </c>
+      <c r="C343" s="7" t="s">
+        <v>979</v>
+      </c>
+      <c r="D343" t="s">
+        <v>815</v>
+      </c>
+      <c r="E343" t="s">
+        <v>201</v>
+      </c>
+      <c r="F343">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A344" s="5" t="s">
+        <v>799</v>
+      </c>
+      <c r="B344" s="6" t="s">
+        <v>890</v>
+      </c>
+      <c r="C344" s="7" t="s">
+        <v>980</v>
+      </c>
+      <c r="D344" t="s">
+        <v>815</v>
+      </c>
+      <c r="E344" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="F344">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A345" s="5" t="s">
+        <v>800</v>
+      </c>
+      <c r="B345" s="6" t="s">
+        <v>891</v>
+      </c>
+      <c r="C345" s="7" t="s">
+        <v>981</v>
+      </c>
+      <c r="D345" t="s">
+        <v>815</v>
+      </c>
+      <c r="E345" t="s">
+        <v>203</v>
+      </c>
+      <c r="F345">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A346" s="5" t="s">
+        <v>801</v>
+      </c>
+      <c r="B346" s="6" t="s">
+        <v>892</v>
+      </c>
+      <c r="C346" s="7" t="s">
+        <v>982</v>
+      </c>
+      <c r="D346" t="s">
+        <v>815</v>
+      </c>
+      <c r="E346" t="s">
+        <v>204</v>
+      </c>
+      <c r="F346">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A347" s="5" t="s">
+        <v>802</v>
+      </c>
+      <c r="B347" s="6" t="s">
+        <v>893</v>
+      </c>
+      <c r="C347" s="7" t="s">
+        <v>983</v>
+      </c>
+      <c r="D347" t="s">
+        <v>815</v>
+      </c>
+      <c r="E347" t="s">
+        <v>205</v>
+      </c>
+      <c r="F347">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A348" s="5" t="s">
+        <v>803</v>
+      </c>
+      <c r="B348" s="6" t="s">
+        <v>894</v>
+      </c>
+      <c r="C348" s="7" t="s">
+        <v>984</v>
+      </c>
+      <c r="D348" t="s">
+        <v>815</v>
+      </c>
+      <c r="E348" t="s">
+        <v>206</v>
+      </c>
+      <c r="F348">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A349" s="5" t="s">
+        <v>804</v>
+      </c>
+      <c r="B349" s="6" t="s">
+        <v>895</v>
+      </c>
+      <c r="C349" s="7" t="s">
+        <v>985</v>
+      </c>
+      <c r="D349" t="s">
+        <v>815</v>
+      </c>
+      <c r="E349" t="s">
+        <v>207</v>
+      </c>
+      <c r="F349">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A350" s="5" t="s">
+        <v>805</v>
+      </c>
+      <c r="B350" s="6" t="s">
+        <v>896</v>
+      </c>
+      <c r="C350" s="7" t="s">
+        <v>986</v>
+      </c>
+      <c r="D350" t="s">
+        <v>815</v>
+      </c>
+      <c r="E350" t="s">
+        <v>208</v>
+      </c>
+      <c r="F350">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A351" s="5" t="s">
+        <v>806</v>
+      </c>
+      <c r="B351" s="6" t="s">
+        <v>897</v>
+      </c>
+      <c r="C351" s="7" t="s">
+        <v>987</v>
+      </c>
+      <c r="D351" t="s">
+        <v>815</v>
+      </c>
+      <c r="E351" t="s">
+        <v>209</v>
+      </c>
+      <c r="F351">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A352" s="5" t="s">
+        <v>807</v>
+      </c>
+      <c r="B352" s="6" t="s">
+        <v>898</v>
+      </c>
+      <c r="C352" s="7" t="s">
+        <v>988</v>
+      </c>
+      <c r="D352" t="s">
+        <v>815</v>
+      </c>
+      <c r="E352" t="s">
+        <v>210</v>
+      </c>
+      <c r="F352">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A353" s="5" t="s">
+        <v>808</v>
+      </c>
+      <c r="B353" s="6" t="s">
+        <v>899</v>
+      </c>
+      <c r="C353" s="7" t="s">
+        <v>989</v>
+      </c>
+      <c r="D353" t="s">
+        <v>815</v>
+      </c>
+      <c r="E353" t="s">
+        <v>211</v>
+      </c>
+      <c r="F353">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A354" s="5" t="s">
+        <v>809</v>
+      </c>
+      <c r="B354" s="6" t="s">
+        <v>900</v>
+      </c>
+      <c r="C354" s="7" t="s">
+        <v>990</v>
+      </c>
+      <c r="D354" t="s">
+        <v>815</v>
+      </c>
+      <c r="E354" t="s">
+        <v>212</v>
+      </c>
+      <c r="F354">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="355" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A355" s="5" t="s">
+        <v>810</v>
+      </c>
+      <c r="B355" s="6" t="s">
+        <v>901</v>
+      </c>
+      <c r="C355" s="7" t="s">
+        <v>991</v>
+      </c>
+      <c r="D355" t="s">
+        <v>815</v>
+      </c>
+      <c r="E355" t="s">
+        <v>213</v>
+      </c>
+      <c r="F355">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="356" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A356" s="5" t="s">
+        <v>811</v>
+      </c>
+      <c r="B356" s="6" t="s">
+        <v>902</v>
+      </c>
+      <c r="C356" s="7" t="s">
+        <v>992</v>
+      </c>
+      <c r="D356" t="s">
+        <v>815</v>
+      </c>
+      <c r="E356" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="F356">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="357" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A357" s="5" t="s">
+        <v>812</v>
+      </c>
+      <c r="B357" s="6" t="s">
+        <v>903</v>
+      </c>
+      <c r="C357" s="7" t="s">
+        <v>993</v>
+      </c>
+      <c r="D357" t="s">
+        <v>815</v>
+      </c>
+      <c r="E357" t="s">
+        <v>215</v>
+      </c>
+      <c r="F357">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="358" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A358" s="5" t="s">
+        <v>813</v>
+      </c>
+      <c r="B358" s="6" t="s">
+        <v>904</v>
+      </c>
+      <c r="C358" s="7" t="s">
+        <v>994</v>
+      </c>
+      <c r="D358" t="s">
+        <v>815</v>
+      </c>
+      <c r="E358" t="s">
+        <v>216</v>
+      </c>
+      <c r="F358">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="359" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A359" s="5" t="s">
+        <v>814</v>
+      </c>
+      <c r="B359" s="6" t="s">
+        <v>905</v>
+      </c>
+      <c r="C359" s="7" t="s">
+        <v>995</v>
+      </c>
+      <c r="D359" t="s">
+        <v>815</v>
+      </c>
+      <c r="E359" t="s">
+        <v>217</v>
+      </c>
+      <c r="F359">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
Added Rep1 Plate Four and updated relevant files.
</commit_message>
<xml_diff>
--- a/data/Designs/Designs_masterfile.xlsx
+++ b/data/Designs/Designs_masterfile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOL428\Documents\GitHub\SynBioMLMH\SynbioML\data\Designs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HOL428\Documents\Repos\SynbioML\data\Designs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE92575-26FB-445C-B493-41E3612553D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599BF7DC-778D-4540-A0CD-57536132E8B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="3350" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3394,8 +3394,8 @@
   </sheetPr>
   <dimension ref="A1:F359"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A263" workbookViewId="0">
-      <selection activeCell="A271" sqref="A271"/>
+    <sheetView tabSelected="1" topLeftCell="A337" workbookViewId="0">
+      <selection activeCell="D347" sqref="D347"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>